<commit_message>
data upload for PM23, OB23, JI23
</commit_message>
<xml_diff>
--- a/projects_2023/JI23_FIN_SA/JI23_FIN_SA_combined_report.xlsx
+++ b/projects_2023/JI23_FIN_SA/JI23_FIN_SA_combined_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lab-admin\Documents\GitHub\HAL_data\projects_2023\JI23_FIN_SA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1D670B-AEBA-491A-835A-37C201B9A2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEBC6448-0300-47C9-A0CE-D41A85D4B3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11460" yWindow="1005" windowWidth="15195" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JI23_FIN_SA_combined_report" sheetId="1" r:id="rId1"/>
@@ -1045,7 +1045,7 @@
                     <c:v>0.439370492</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>8.6548664140000007</c:v>
+                    <c:v>8.8421803059999995</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1084,7 +1084,7 @@
                     <c:v>0.439370492</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>8.6548664140000007</c:v>
+                    <c:v>8.8421803059999995</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1137,7 +1137,7 @@
                   <c:v>1266.0733130000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>565.48945030000004</c:v>
+                  <c:v>502.50721220000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1176,7 +1176,7 @@
                   <c:v>24.455121080000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>596.58737570000005</c:v>
+                  <c:v>608.69304220000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2213,7 +2213,7 @@
                     <c:v>0.439370492</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>8.6548664140000007</c:v>
+                    <c:v>8.8421803059999995</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2252,7 +2252,7 @@
                     <c:v>0.439370492</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>8.6548664140000007</c:v>
+                    <c:v>8.8421803059999995</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -2305,7 +2305,7 @@
                   <c:v>1266.0733130000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>565.48945030000004</c:v>
+                  <c:v>502.50721220000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2344,7 +2344,7 @@
                   <c:v>24.455121080000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>596.58737570000005</c:v>
+                  <c:v>608.69304220000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2642,7 +2642,7 @@
                   <c:noEndCap val="0"/>
                   <c:plus>
                     <c:numRef>
-                      <c:extLst>
+                      <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                         <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                           <c15:formulaRef>
                             <c15:sqref>JI23_FIN_SA_combined_report!$E$19:$E$22</c15:sqref>
@@ -2669,7 +2669,7 @@
                   </c:plus>
                   <c:minus>
                     <c:numRef>
-                      <c:extLst>
+                      <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                         <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                           <c15:formulaRef>
                             <c15:sqref>JI23_FIN_SA_combined_report!$E$19:$E$22</c15:sqref>
@@ -2710,7 +2710,7 @@
                 </c:errBars>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>JI23_FIN_SA_combined_report!$X$19:$X$22</c15:sqref>
@@ -2737,7 +2737,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>JI23_FIN_SA_combined_report!$D$19:$D$22</c15:sqref>
@@ -2763,7 +2763,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-82D8-43E6-A5CB-7550CB716783}"/>
                   </c:ext>
@@ -2826,7 +2826,7 @@
                   <c:noEndCap val="0"/>
                   <c:plus>
                     <c:numRef>
-                      <c:extLst>
+                      <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                         <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                           <c15:formulaRef>
                             <c15:sqref>JI23_FIN_SA_combined_report!$E$23:$E$30</c15:sqref>
@@ -2865,7 +2865,7 @@
                   </c:plus>
                   <c:minus>
                     <c:numRef>
-                      <c:extLst>
+                      <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                         <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                           <c15:formulaRef>
                             <c15:sqref>JI23_FIN_SA_combined_report!$E$23:$E$30</c15:sqref>
@@ -2918,7 +2918,7 @@
                 </c:errBars>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>JI23_FIN_SA_combined_report!$X$23:$X$30</c15:sqref>
@@ -2957,7 +2957,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>JI23_FIN_SA_combined_report!$D$23:$D$30</c15:sqref>
@@ -2995,7 +2995,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-82D8-43E6-A5CB-7550CB716783}"/>
                   </c:ext>
@@ -3677,7 +3677,7 @@
                           <c:v>0.439370492</c:v>
                         </c:pt>
                         <c:pt idx="9">
-                          <c:v>8.6548664140000007</c:v>
+                          <c:v>8.8421803059999995</c:v>
                         </c:pt>
                       </c:numCache>
                     </c:numRef>
@@ -3722,7 +3722,7 @@
                           <c:v>0.439370492</c:v>
                         </c:pt>
                         <c:pt idx="9">
-                          <c:v>8.6548664140000007</c:v>
+                          <c:v>8.8421803059999995</c:v>
                         </c:pt>
                       </c:numCache>
                     </c:numRef>
@@ -3781,7 +3781,7 @@
                         <c:v>1266.0733130000001</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>565.48945030000004</c:v>
+                        <c:v>502.50721220000003</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3826,7 +3826,7 @@
                         <c:v>24.455121080000001</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>596.58737570000005</c:v>
+                        <c:v>608.69304220000004</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -4896,7 +4896,7 @@
                           <c:v>0.439370492</c:v>
                         </c:pt>
                         <c:pt idx="9">
-                          <c:v>8.6548664140000007</c:v>
+                          <c:v>8.8421803059999995</c:v>
                         </c:pt>
                       </c:numCache>
                     </c:numRef>
@@ -4941,7 +4941,7 @@
                           <c:v>0.439370492</c:v>
                         </c:pt>
                         <c:pt idx="9">
-                          <c:v>8.6548664140000007</c:v>
+                          <c:v>8.8421803059999995</c:v>
                         </c:pt>
                       </c:numCache>
                     </c:numRef>
@@ -5000,7 +5000,7 @@
                         <c:v>1266.0733130000001</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>565.48945030000004</c:v>
+                        <c:v>502.50721220000003</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -5045,7 +5045,7 @@
                         <c:v>24.455121080000001</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>596.58737570000005</c:v>
+                        <c:v>608.69304220000004</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -6196,7 +6196,7 @@
                           <c:v>0.439370492</c:v>
                         </c:pt>
                         <c:pt idx="9">
-                          <c:v>8.6548664140000007</c:v>
+                          <c:v>8.8421803059999995</c:v>
                         </c:pt>
                       </c:numCache>
                     </c:numRef>
@@ -6241,7 +6241,7 @@
                           <c:v>0.439370492</c:v>
                         </c:pt>
                         <c:pt idx="9">
-                          <c:v>8.6548664140000007</c:v>
+                          <c:v>8.8421803059999995</c:v>
                         </c:pt>
                       </c:numCache>
                     </c:numRef>
@@ -6300,7 +6300,7 @@
                         <c:v>1266.0733130000001</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>565.48945030000004</c:v>
+                        <c:v>502.50721220000003</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -6345,7 +6345,7 @@
                         <c:v>24.455121080000001</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>596.58737570000005</c:v>
+                        <c:v>608.69304220000004</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -10353,8 +10353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y15" sqref="Y15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11080,19 +11080,19 @@
         <v>42</v>
       </c>
       <c r="D11" s="2">
-        <v>596.58737570000005</v>
+        <v>608.69304220000004</v>
       </c>
       <c r="E11" s="2">
-        <v>8.6548664140000007</v>
+        <v>8.8421803059999995</v>
       </c>
       <c r="F11" s="2">
-        <v>1.4507290580000001</v>
+        <v>1.4526501359999999</v>
       </c>
       <c r="G11" s="2">
-        <v>35.961680180000002</v>
+        <v>34.299511559999999</v>
       </c>
       <c r="H11" s="2">
-        <v>0.67179100300000005</v>
+        <v>0.65766885799999997</v>
       </c>
       <c r="I11" s="2">
         <v>408.0253045</v>
@@ -11128,19 +11128,19 @@
         <v>4.9325280000000003E-3</v>
       </c>
       <c r="T11" s="3">
-        <v>1.02E-6</v>
+        <v>1.1400000000000001E-6</v>
       </c>
       <c r="U11" s="2">
-        <v>550.19655479999994</v>
+        <v>488.91758579999998</v>
       </c>
       <c r="V11" s="2">
-        <v>65.076151370000005</v>
+        <v>57.828197119999999</v>
       </c>
       <c r="W11" s="2">
         <v>0</v>
       </c>
       <c r="X11" s="2">
-        <v>565.48945030000004</v>
+        <v>502.50721220000003</v>
       </c>
     </row>
     <row r="12" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>